<commit_message>
DSSR and ADFD+ updated.
</commit_message>
<xml_diff>
--- a/papers/ADFDPlus/ADFD+ vs Randoop.xlsx
+++ b/papers/ADFDPlus/ADFD+ vs Randoop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16580" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22520" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="66">
   <si>
     <t>ADFD+</t>
   </si>
@@ -189,21 +189,6 @@
     <t>Domain</t>
   </si>
   <si>
-    <t>Point</t>
-  </si>
-  <si>
-    <t>Block</t>
-  </si>
-  <si>
-    <t>Strip</t>
-  </si>
-  <si>
-    <t>Average time taken by Randoop</t>
-  </si>
-  <si>
-    <t>Average Test cases by Randoop</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
@@ -216,10 +201,25 @@
     <t>one dim block time</t>
   </si>
   <si>
-    <t>Average test cases by ADFD+</t>
+    <t>Average time taken by</t>
   </si>
   <si>
-    <t>Average time taken by ADFD+</t>
+    <t xml:space="preserve">Average time taken by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average test cases by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Test cases by </t>
+  </si>
+  <si>
+    <t>Point failure</t>
+  </si>
+  <si>
+    <t>Block failure</t>
+  </si>
+  <si>
+    <t>Strip failure</t>
   </si>
 </sst>
 </file>
@@ -227,7 +227,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -512,14 +512,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -981,11 +981,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="601307512"/>
-        <c:axId val="138156504"/>
+        <c:axId val="618399864"/>
+        <c:axId val="618403064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="601307512"/>
+        <c:axId val="618399864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -994,7 +994,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138156504"/>
+        <c:crossAx val="618403064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1002,7 +1002,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="138156504"/>
+        <c:axId val="618403064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1012,7 +1012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="601307512"/>
+        <c:crossAx val="618399864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1043,11 +1043,22 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.241354800799154"/>
+          <c:y val="0.0561056105610561"/>
+          <c:w val="0.677261957926901"/>
+          <c:h val="0.735842103895429"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1058,78 +1069,37 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average test cases by ADFD+</c:v>
+                  <c:v>ADFD+</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Results!$I$19:$K$24</c:f>
-              <c:multiLvlStrCache>
+            <c:strRef>
+              <c:f>Results!$I$19:$I$24</c:f>
+              <c:strCache>
                 <c:ptCount val="6"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Point</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Point</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Block</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Block</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Strip</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Strip</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>One</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Two</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>One</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Two</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>One</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Two</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Pro1</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Pro2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Pro3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Pro4</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Pro5</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Pro6</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+                <c:pt idx="0">
+                  <c:v>Pro1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pro2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pro3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Pro4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Pro5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Pro6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1158,7 +1128,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1169,78 +1138,37 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average Test cases by Randoop</c:v>
+                  <c:v>Randoop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Results!$I$19:$K$24</c:f>
-              <c:multiLvlStrCache>
+            <c:strRef>
+              <c:f>Results!$I$19:$I$24</c:f>
+              <c:strCache>
                 <c:ptCount val="6"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Point</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Point</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Block</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Block</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Strip</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Strip</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>One</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Two</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>One</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Two</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>One</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Two</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Pro1</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Pro2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Pro3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Pro4</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Pro5</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Pro6</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+                <c:pt idx="0">
+                  <c:v>Pro1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pro2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pro3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Pro4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Pro5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Pro6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1269,7 +1197,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1279,13 +1206,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="734380472"/>
-        <c:axId val="724548664"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="614384888"/>
+        <c:axId val="614387864"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="734380472"/>
+        <c:axId val="614384888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1294,7 +1220,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="724548664"/>
+        <c:crossAx val="614387864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1302,25 +1228,64 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="724548664"/>
+        <c:axId val="614387864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Numbe</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>r of Test Cases</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.063931447128431"/>
+              <c:y val="0.28324731685767"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="734380472"/>
+        <c:crossAx val="614384888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.346824814271097"/>
+          <c:y val="0.10341311296484"/>
+          <c:w val="0.156815694648338"/>
+          <c:h val="0.132560484394896"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1605,11 +1570,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="720425368"/>
-        <c:axId val="601489240"/>
+        <c:axId val="614044728"/>
+        <c:axId val="614047928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="720425368"/>
+        <c:axId val="614044728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1618,7 +1583,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="601489240"/>
+        <c:crossAx val="614047928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1626,7 +1591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="601489240"/>
+        <c:axId val="614047928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,7 +1601,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="720425368"/>
+        <c:crossAx val="614044728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1923,11 +1888,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="601664392"/>
-        <c:axId val="601666056"/>
+        <c:axId val="614084536"/>
+        <c:axId val="614087736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="601664392"/>
+        <c:axId val="614084536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1936,7 +1901,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="601666056"/>
+        <c:crossAx val="614087736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1944,7 +1909,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="601666056"/>
+        <c:axId val="614087736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1954,7 +1919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="601664392"/>
+        <c:crossAx val="614084536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2231,11 +2196,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="601390296"/>
-        <c:axId val="601338248"/>
+        <c:axId val="614125128"/>
+        <c:axId val="614128328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="601390296"/>
+        <c:axId val="614125128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2244,7 +2209,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="601338248"/>
+        <c:crossAx val="614128328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2252,7 +2217,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="601338248"/>
+        <c:axId val="614128328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2262,7 +2227,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="601390296"/>
+        <c:crossAx val="614125128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2539,11 +2504,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="720480840"/>
-        <c:axId val="720464456"/>
+        <c:axId val="614166216"/>
+        <c:axId val="614169416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="720480840"/>
+        <c:axId val="614166216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2552,7 +2517,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="720464456"/>
+        <c:crossAx val="614169416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2560,7 +2525,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="720464456"/>
+        <c:axId val="614169416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2570,7 +2535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="720480840"/>
+        <c:crossAx val="614166216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2847,11 +2812,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="601511688"/>
-        <c:axId val="601697416"/>
+        <c:axId val="614207528"/>
+        <c:axId val="614210728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="601511688"/>
+        <c:axId val="614207528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2860,7 +2825,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="601697416"/>
+        <c:crossAx val="614210728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2868,7 +2833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="601697416"/>
+        <c:axId val="614210728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2878,7 +2843,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="601511688"/>
+        <c:crossAx val="614207528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3451,11 +3416,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="601474216"/>
-        <c:axId val="601479816"/>
+        <c:axId val="614224888"/>
+        <c:axId val="614228120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="601474216"/>
+        <c:axId val="614224888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3474,7 +3439,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="601479816"/>
+        <c:crossAx val="614228120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3482,7 +3447,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="601479816"/>
+        <c:axId val="614228120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3504,14 +3469,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="601474216"/>
+        <c:crossAx val="614224888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4080,11 +4044,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="601555000"/>
-        <c:axId val="601535208"/>
+        <c:axId val="614311368"/>
+        <c:axId val="614314536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="601555000"/>
+        <c:axId val="614311368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4103,7 +4067,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="601535208"/>
+        <c:crossAx val="614314536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4111,7 +4075,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="601535208"/>
+        <c:axId val="614314536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4133,14 +4097,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="601555000"/>
+        <c:crossAx val="614311368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4173,9 +4136,20 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.198706441068235"/>
+          <c:y val="0.0489252750690932"/>
+          <c:w val="0.733920603674541"/>
+          <c:h val="0.733193535018649"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -4186,78 +4160,37 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average time taken by ADFD+</c:v>
+                  <c:v>ADFD+</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Results!$I$19:$K$24</c:f>
-              <c:multiLvlStrCache>
+            <c:strRef>
+              <c:f>Results!$I$19:$I$24</c:f>
+              <c:strCache>
                 <c:ptCount val="6"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Point</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Point</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Block</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Block</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Strip</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Strip</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>One</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Two</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>One</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Two</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>One</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Two</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Pro1</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Pro2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Pro3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Pro4</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Pro5</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Pro6</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+                <c:pt idx="0">
+                  <c:v>Pro1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pro2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pro3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Pro4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Pro5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Pro6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -4286,7 +4219,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4297,78 +4229,37 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average time taken by Randoop</c:v>
+                  <c:v>Randoop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Results!$I$19:$K$24</c:f>
-              <c:multiLvlStrCache>
+            <c:strRef>
+              <c:f>Results!$I$19:$I$24</c:f>
+              <c:strCache>
                 <c:ptCount val="6"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Point</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Point</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Block</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Block</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Strip</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Strip</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>One</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Two</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>One</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Two</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>One</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Two</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Pro1</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Pro2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Pro3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Pro4</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Pro5</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Pro6</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+                <c:pt idx="0">
+                  <c:v>Pro1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pro2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pro3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Pro4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Pro5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Pro6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -4397,7 +4288,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4407,13 +4297,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="634239464"/>
-        <c:axId val="633985160"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="614350520"/>
+        <c:axId val="614353496"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="634239464"/>
+        <c:axId val="614350520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4422,7 +4311,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="633985160"/>
+        <c:crossAx val="614353496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4430,25 +4319,64 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="633985160"/>
+        <c:axId val="614353496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CPU</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time (sec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0439392693406797"/>
+              <c:y val="0.336051780779058"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="634239464"/>
+        <c:crossAx val="614350520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.721457823646718"/>
+          <c:y val="0.0866616259060333"/>
+          <c:w val="0.144941921424313"/>
+          <c:h val="0.132999426396204"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4722,16 +4650,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4752,16 +4680,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5117,30 +5045,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:27">
-      <c r="D1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="8"/>
-      <c r="H1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="8"/>
-      <c r="L1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="M1" s="8"/>
-      <c r="P1" s="8" t="s">
+      <c r="D1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="H1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="10"/>
+      <c r="L1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="10"/>
+      <c r="P1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="8"/>
-      <c r="T1" s="8" t="s">
+      <c r="Q1" s="10"/>
+      <c r="T1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="8"/>
-      <c r="Z1" s="8" t="s">
+      <c r="U1" s="10"/>
+      <c r="Z1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="8"/>
+      <c r="AA1" s="10"/>
     </row>
     <row r="2" spans="4:27">
       <c r="D2" s="1" t="s">
@@ -6430,8 +6358,8 @@
         <f t="shared" si="0"/>
         <v>12619</v>
       </c>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
       <c r="L34" s="1">
         <f>MIN(L3:L33)</f>
         <v>2</v>
@@ -6495,8 +6423,8 @@
         <f t="shared" si="3"/>
         <v>15008.5</v>
       </c>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
       <c r="L35" s="1">
         <f t="shared" ref="L35:M35" si="4">QUARTILE(L3:L32,1)</f>
         <v>3</v>
@@ -6560,8 +6488,8 @@
         <f t="shared" si="7"/>
         <v>15825</v>
       </c>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
       <c r="L36" s="1">
         <f t="shared" ref="L36:M36" si="8">MEDIAN(L3:L32)</f>
         <v>3</v>
@@ -6625,8 +6553,8 @@
         <f t="shared" si="11"/>
         <v>16647.5</v>
       </c>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
       <c r="L37" s="1">
         <f t="shared" ref="L37:M37" si="12">QUARTILE(L3:L32,3)</f>
         <v>4</v>
@@ -6690,8 +6618,8 @@
         <f t="shared" si="15"/>
         <v>17632</v>
       </c>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
       <c r="L38" s="1">
         <f t="shared" ref="L38:M38" si="16">MAX(L3:L32)</f>
         <v>5</v>
@@ -7163,7 +7091,7 @@
     </row>
     <row r="72" spans="3:36">
       <c r="C72" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D72">
         <f>AVERAGE(D3:D32)</f>
@@ -7339,30 +7267,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9" t="s">
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9" t="s">
+      <c r="M1" s="11"/>
+      <c r="N1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="9"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="2:15">
       <c r="D2" s="4" t="s">
@@ -9130,7 +9058,7 @@
     </row>
     <row r="46" spans="3:15">
       <c r="C46" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D46">
         <f>AVERAGE(D3:D32)</f>
@@ -9218,30 +9146,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9" t="s">
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9" t="s">
+      <c r="M1" s="11"/>
+      <c r="N1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="9"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="2:15">
       <c r="D2" s="4" t="s">
@@ -10998,7 +10926,7 @@
     <row r="47" spans="1:15" ht="15" customHeight="1"/>
     <row r="48" spans="1:15">
       <c r="C48" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D48">
         <f>AVERAGE(D3:D32)</f>
@@ -11071,10 +10999,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="I18:O24"/>
+  <dimension ref="I17:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11084,6 +11012,20 @@
     <col min="15" max="15" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="17" spans="9:15">
+      <c r="L17" t="s">
+        <v>59</v>
+      </c>
+      <c r="M17" t="s">
+        <v>60</v>
+      </c>
+      <c r="N17" t="s">
+        <v>61</v>
+      </c>
+      <c r="O17" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="18" spans="9:15">
       <c r="I18" t="s">
         <v>44</v>
@@ -11095,16 +11037,16 @@
         <v>54</v>
       </c>
       <c r="L18" t="s">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="M18" t="s">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="9:15">
@@ -11115,18 +11057,18 @@
         <v>52</v>
       </c>
       <c r="K19" t="s">
-        <v>55</v>
-      </c>
-      <c r="L19" s="10">
+        <v>63</v>
+      </c>
+      <c r="L19" s="8">
         <v>3.9666666666666668</v>
       </c>
-      <c r="M19" s="11">
+      <c r="M19" s="9">
         <v>178.96666666666667</v>
       </c>
-      <c r="N19" s="11">
+      <c r="N19" s="9">
         <v>5545.4666666666662</v>
       </c>
-      <c r="O19" s="11">
+      <c r="O19" s="9">
         <v>11622.933333333332</v>
       </c>
     </row>
@@ -11138,18 +11080,18 @@
         <v>53</v>
       </c>
       <c r="K20" t="s">
-        <v>55</v>
-      </c>
-      <c r="L20" s="10">
+        <v>63</v>
+      </c>
+      <c r="L20" s="8">
         <v>2.2666666666666666</v>
       </c>
-      <c r="M20" s="11">
+      <c r="M20" s="9">
         <v>168.76666666666668</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="9">
         <v>3658.4</v>
       </c>
-      <c r="O20" s="11">
+      <c r="O20" s="9">
         <v>9926.2333333333336</v>
       </c>
     </row>
@@ -11161,18 +11103,18 @@
         <v>52</v>
       </c>
       <c r="K21" t="s">
-        <v>56</v>
-      </c>
-      <c r="L21" s="10">
+        <v>64</v>
+      </c>
+      <c r="L21" s="8">
         <v>2.1333333333333333</v>
       </c>
-      <c r="M21" s="11">
+      <c r="M21" s="9">
         <v>155.93333333333334</v>
       </c>
-      <c r="N21" s="11">
+      <c r="N21" s="9">
         <v>3100.6333333333332</v>
       </c>
-      <c r="O21" s="11">
+      <c r="O21" s="9">
         <v>9270.5333333333328</v>
       </c>
     </row>
@@ -11184,18 +11126,18 @@
         <v>53</v>
       </c>
       <c r="K22" t="s">
-        <v>56</v>
-      </c>
-      <c r="L22" s="10">
+        <v>64</v>
+      </c>
+      <c r="L22" s="8">
         <v>6.6</v>
       </c>
-      <c r="M22" s="11">
+      <c r="M22" s="9">
         <v>83.466666666666669</v>
       </c>
-      <c r="N22" s="11">
+      <c r="N22" s="9">
         <v>6578.2666666666664</v>
       </c>
-      <c r="O22" s="11">
+      <c r="O22" s="9">
         <v>15705.533333333333</v>
       </c>
     </row>
@@ -11207,18 +11149,18 @@
         <v>52</v>
       </c>
       <c r="K23" t="s">
-        <v>57</v>
-      </c>
-      <c r="L23" s="10">
+        <v>65</v>
+      </c>
+      <c r="L23" s="8">
         <v>3.2666666666666666</v>
       </c>
-      <c r="M23" s="11">
+      <c r="M23" s="9">
         <v>77.8</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N23" s="9">
         <v>4741.7</v>
       </c>
-      <c r="O23" s="11">
+      <c r="O23" s="9">
         <v>14724.533333333333</v>
       </c>
     </row>
@@ -11230,18 +11172,18 @@
         <v>53</v>
       </c>
       <c r="K24" t="s">
-        <v>57</v>
-      </c>
-      <c r="L24" s="10">
+        <v>65</v>
+      </c>
+      <c r="L24" s="8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="M24" s="11">
+      <c r="M24" s="9">
         <v>70.933333333333337</v>
       </c>
-      <c r="N24" s="11">
+      <c r="N24" s="9">
         <v>4047.7</v>
       </c>
-      <c r="O24" s="11">
+      <c r="O24" s="9">
         <v>14513.533333333333</v>
       </c>
     </row>

</xml_diff>